<commit_message>
Added missing norm uncertainties to some sia and sidis tables and added additional sia hadron datasets
</commit_message>
<xml_diff>
--- a/sia/expdata/4003.xlsx
+++ b/sia/expdata/4003.xlsx
@@ -450,7 +450,7 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E2">
         <v>0.02</v>
@@ -479,7 +479,7 @@
         <v>10</v>
       </c>
       <c r="D3">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E3">
         <v>0.05</v>
@@ -508,7 +508,7 @@
         <v>10</v>
       </c>
       <c r="D4">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E4">
         <v>0.1</v>
@@ -537,7 +537,7 @@
         <v>10</v>
       </c>
       <c r="D5">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E5">
         <v>0.2</v>
@@ -566,7 +566,7 @@
         <v>10</v>
       </c>
       <c r="D6">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E6">
         <v>0.3</v>
@@ -595,7 +595,7 @@
         <v>10</v>
       </c>
       <c r="D7">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E7">
         <v>0.4</v>
@@ -624,7 +624,7 @@
         <v>10</v>
       </c>
       <c r="D8">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E8">
         <v>0.5</v>

</xml_diff>